<commit_message>
Added software libraries for onstep as well as the configured code required to upload to esp32. Also included some Arduino libraries
</commit_message>
<xml_diff>
--- a/KiCad/Stardust/bom.xlsx
+++ b/KiCad/Stardust/bom.xlsx
@@ -5,23 +5,36 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bosleis\Documents\Stardust\KiCad\Stardust\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/af248ad19860a01a/Documents/Stardust/KiCad/Stardust/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A225B4CA-49FC-45AE-A0A9-B8C6435F50CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:9_{A225B4CA-49FC-45AE-A0A9-B8C6435F50CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4B398BE-FC29-4D11-A01D-66C13F99369D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{94A0EDEC-EB08-4B5B-A3BB-2FB460776BAA}"/>
+    <workbookView xWindow="38820" yWindow="4545" windowWidth="26820" windowHeight="12525" xr2:uid="{94A0EDEC-EB08-4B5B-A3BB-2FB460776BAA}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="2" r:id="rId1"/>
     <sheet name="items" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>C5</t>
   </si>
@@ -252,6 +265,21 @@
   </si>
   <si>
     <t>KAM21BR71H104JT</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Ordered?</t>
   </si>
 </sst>
 </file>
@@ -1141,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15A279D-0970-445D-B90F-EE6C1070B374}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,7 +1182,7 @@
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>69</v>
@@ -1171,8 +1199,20 @@
       <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1189,8 +1229,14 @@
         <f>D2*E2</f>
         <v>0.52</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>39</v>
       </c>
@@ -1207,8 +1253,14 @@
         <f t="shared" ref="F3:F17" si="0">D3*E3</f>
         <v>0.23</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>75</v>
       </c>
@@ -1225,8 +1277,14 @@
         <f t="shared" si="0"/>
         <v>1.28</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="J4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>40</v>
       </c>
@@ -1243,8 +1301,14 @@
         <f t="shared" si="0"/>
         <v>1.78</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>77</v>
+      </c>
+      <c r="J5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>41</v>
       </c>
@@ -1261,8 +1325,14 @@
         <f t="shared" si="0"/>
         <v>0.49</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>46</v>
       </c>
@@ -1279,8 +1349,14 @@
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>77</v>
+      </c>
+      <c r="J7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>66</v>
       </c>
@@ -1297,8 +1373,14 @@
         <f t="shared" si="0"/>
         <v>1.21</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -1315,8 +1397,14 @@
         <f t="shared" si="0"/>
         <v>0.97</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>77</v>
+      </c>
+      <c r="J9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>49</v>
       </c>
@@ -1333,8 +1421,14 @@
         <f t="shared" si="0"/>
         <v>3.2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>50</v>
       </c>
@@ -1351,8 +1445,14 @@
         <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>52</v>
       </c>
@@ -1369,8 +1469,14 @@
         <f t="shared" si="0"/>
         <v>1.05</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>77</v>
+      </c>
+      <c r="J12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>68</v>
       </c>
@@ -1387,8 +1493,14 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>77</v>
+      </c>
+      <c r="J13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>70</v>
       </c>
@@ -1405,8 +1517,14 @@
         <f t="shared" si="0"/>
         <v>4.8099999999999996</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>43</v>
       </c>
@@ -1423,8 +1541,14 @@
         <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>44</v>
       </c>
@@ -1441,8 +1565,14 @@
         <f t="shared" si="0"/>
         <v>1.32</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>73</v>
       </c>
@@ -1459,8 +1589,14 @@
         <f t="shared" si="0"/>
         <v>22.99</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>77</v>
+      </c>
+      <c r="J17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F19" s="4">
         <f>SUM(F2:F17)</f>
         <v>51.66</v>

</xml_diff>